<commit_message>
Deploy e630299 from branch develop
</commit_message>
<xml_diff>
--- a/public/embedded/3-5-1.xlsx
+++ b/public/embedded/3-5-1.xlsx
@@ -16,12 +16,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>A</t>
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>Diff</t>
   </si>
 </sst>
 </file>
@@ -91,8 +94,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -108,9 +111,9 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:spPr>
+            <a:noFill/>
+          </c:spPr>
           <c:cat>
             <c:numRef>
               <c:f>Tabelle1!$A$2:$A$8</c:f>
@@ -171,7 +174,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -187,9 +189,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>Tabelle1!$A$2:$A$8</c:f>
@@ -222,35 +221,34 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$C$2:$C$8</c:f>
+              <c:f>Tabelle1!$D$2:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>254</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>272</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>258</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>253</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>272</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>266</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>265</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -260,13 +258,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="44107776"/>
-        <c:axId val="44340288"/>
-      </c:lineChart>
+        <c:axId val="181815296"/>
+        <c:axId val="93013696"/>
+      </c:areaChart>
       <c:catAx>
-        <c:axId val="44107776"/>
+        <c:axId val="181815296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -276,7 +272,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44340288"/>
+        <c:crossAx val="93013696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -284,7 +280,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44340288"/>
+        <c:axId val="93013696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -295,9 +291,9 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44107776"/>
+        <c:crossAx val="181815296"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -634,23 +630,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2010</v>
       </c>
@@ -660,8 +659,12 @@
       <c r="C2">
         <v>254</v>
       </c>
+      <c r="D2">
+        <f>C2-B2</f>
+        <v>40</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2011</v>
       </c>
@@ -671,8 +674,12 @@
       <c r="C3">
         <v>272</v>
       </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D8" si="0">C3-B3</f>
+        <v>43</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2012</v>
       </c>
@@ -682,8 +689,12 @@
       <c r="C4">
         <v>258</v>
       </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2013</v>
       </c>
@@ -693,8 +704,12 @@
       <c r="C5">
         <v>253</v>
       </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2014</v>
       </c>
@@ -704,8 +719,12 @@
       <c r="C6">
         <v>272</v>
       </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2015</v>
       </c>
@@ -715,8 +734,12 @@
       <c r="C7">
         <v>266</v>
       </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2016</v>
       </c>
@@ -725,6 +748,10 @@
       </c>
       <c r="C8">
         <v>265</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>